<commit_message>
cluster analysis with two groups
-some small trends can be seen, especially between areas
-only two groups were used
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/1_groups_area_time.xlsx
+++ b/_CLUSTER/groups_time_area/1_groups_area_time.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_CLUSTER\groups_time_area\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4715B80-E79A-41DF-A4D8-6E091B22CCDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6EE89F-6F2D-4087-AAC3-7C7AEC0B9FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BCF02780-D300-43E8-921C-29E8CAC5991E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCF02780-D300-43E8-921C-29E8CAC5991E}"/>
   </bookViews>
   <sheets>
-    <sheet name="3_groups" sheetId="1" r:id="rId1"/>
-    <sheet name="4_groups" sheetId="3" r:id="rId2"/>
-    <sheet name="6_groups" sheetId="4" r:id="rId3"/>
+    <sheet name="2_groups" sheetId="5" r:id="rId1"/>
+    <sheet name="3_groups" sheetId="1" r:id="rId2"/>
+    <sheet name="4_groups" sheetId="3" r:id="rId3"/>
+    <sheet name="6_groups" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="55">
   <si>
     <t>Area1</t>
   </si>
@@ -186,6 +187,21 @@
   <si>
     <t>Area5_tot</t>
   </si>
+  <si>
+    <t>area1</t>
+  </si>
+  <si>
+    <t>area2</t>
+  </si>
+  <si>
+    <t>area3</t>
+  </si>
+  <si>
+    <t>Area_J</t>
+  </si>
+  <si>
+    <t>Area4+5</t>
+  </si>
 </sst>
 </file>
 
@@ -305,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -348,6 +364,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -661,11 +680,1513 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E362FAB3-749B-42AE-A5DF-A65E9F55F37B}">
+  <dimension ref="A1:AB50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA52" sqref="AA52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" customWidth="1"/>
+    <col min="16" max="16" width="5.77734375" customWidth="1"/>
+    <col min="18" max="18" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+    <col min="20" max="20" width="6.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>253</v>
+      </c>
+      <c r="D3">
+        <f>C3/$C$5*100</f>
+        <v>53.944562899786789</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>234</v>
+      </c>
+      <c r="H3">
+        <f>G3/$G$5*100</f>
+        <v>78.523489932885909</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>430</v>
+      </c>
+      <c r="L3">
+        <f>K3/$K$5*100</f>
+        <v>68.253968253968253</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>37</v>
+      </c>
+      <c r="T3">
+        <f>S3/$S$5*100</f>
+        <v>64.912280701754383</v>
+      </c>
+      <c r="V3" s="7">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>C3+G3+K3+O3+S3</f>
+        <v>957</v>
+      </c>
+      <c r="X3">
+        <f>W3/$W$5*100</f>
+        <v>65.682910089224436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>216</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D5" si="0">C4/$C$5*100</f>
+        <v>46.055437100213219</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>64</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H5" si="1">G4/$G$5*100</f>
+        <v>21.476510067114095</v>
+      </c>
+      <c r="J4" s="4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>200</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L5" si="2">K4/$K$5*100</f>
+        <v>31.746031746031743</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>20</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T5" si="3">S4/$S$5*100</f>
+        <v>35.087719298245609</v>
+      </c>
+      <c r="V4" s="7">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W5" si="4">C4+G4+K4+O4+S4</f>
+        <v>500</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X5" si="5">W4/$W$5*100</f>
+        <v>34.317089910775564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
+        <f>SUM(C3:C4)</f>
+        <v>469</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G5" s="1">
+        <f>SUM(G3:G4)</f>
+        <v>298</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="K5" s="1">
+        <f>SUM(K3:K4)</f>
+        <v>630</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="S5" s="1">
+        <f>SUM(S3:S4)</f>
+        <v>57</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="4"/>
+        <v>1457</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f>G10/$G$12*100</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>406</v>
+      </c>
+      <c r="L10">
+        <f>K10/$K$12*100</f>
+        <v>56.783216783216787</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>178</v>
+      </c>
+      <c r="P10">
+        <f>O10/$O$12*100</f>
+        <v>56.507936507936506</v>
+      </c>
+      <c r="V10" s="7">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f>C10+G10+K10+O10</f>
+        <v>590</v>
+      </c>
+      <c r="X10">
+        <f>W10/$W$12*100</f>
+        <v>56.840077071290942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H12" si="6">G11/$G$12*100</f>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>309</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L12" si="7">K11/$K$12*100</f>
+        <v>43.216783216783213</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>137</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:P12" si="8">O11/$O$12*100</f>
+        <v>43.492063492063494</v>
+      </c>
+      <c r="V11" s="7">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <f t="shared" ref="W11:W12" si="9">C11+G11+K11+O11</f>
+        <v>448</v>
+      </c>
+      <c r="X11">
+        <f t="shared" ref="X11:X12" si="10">W11/$W$12*100</f>
+        <v>43.159922928709058</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="K12" s="1">
+        <f>SUM(K10:K11)</f>
+        <v>715</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="O12" s="1">
+        <f>SUM(O10:O11)</f>
+        <v>315</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="9"/>
+        <v>1038</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="W16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>57</v>
+      </c>
+      <c r="H17">
+        <f>G17/$G$19*100</f>
+        <v>57.575757575757578</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>513</v>
+      </c>
+      <c r="L17">
+        <f>K17/$K$19*100</f>
+        <v>51.197604790419163</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <f>O17/$O$19*100</f>
+        <v>85.714285714285708</v>
+      </c>
+      <c r="V17" s="7">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f>C17+G17+K17+O17</f>
+        <v>577</v>
+      </c>
+      <c r="X17">
+        <f>W17/$W$19*100</f>
+        <v>52.028854824165919</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>42</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H19" si="11">G18/$G$19*100</f>
+        <v>42.424242424242422</v>
+      </c>
+      <c r="J18" s="4">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>489</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L19" si="12">K18/$K$19*100</f>
+        <v>48.802395209580837</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18:P19" si="13">O18/$O$19*100</f>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="V18" s="7">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <f t="shared" ref="W18:W19" si="14">C18+G18+K18+O18</f>
+        <v>532</v>
+      </c>
+      <c r="X18">
+        <f t="shared" ref="X18:X19" si="15">W18/$W$19*100</f>
+        <v>47.971145175834081</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="G19" s="1">
+        <f>SUM(G17:G18)</f>
+        <v>99</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+      <c r="K19" s="1">
+        <f>SUM(K17:K18)</f>
+        <v>1002</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="12"/>
+        <v>100</v>
+      </c>
+      <c r="O19" s="1">
+        <f>SUM(O17:O18)</f>
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="14"/>
+        <v>1109</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="W24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="X24" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>214</v>
+      </c>
+      <c r="H25">
+        <f>G25/$G$27*100</f>
+        <v>46.929824561403507</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>33.33</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>8</v>
+      </c>
+      <c r="P25">
+        <f>O25/$O$27*100</f>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="V25" s="7">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f>C25+G25+K25+O25</f>
+        <v>223</v>
+      </c>
+      <c r="X25">
+        <f>W25/$W$27*100</f>
+        <v>46.94736842105263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>242</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ref="H26:H27" si="16">G26/$G$27*100</f>
+        <v>53.070175438596493</v>
+      </c>
+      <c r="J26" s="4">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>66.67</v>
+      </c>
+      <c r="N26" s="4">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>7</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ref="P26:P27" si="17">O26/$O$27*100</f>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="V26" s="7">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <f t="shared" ref="W26:W27" si="18">C26+G26+K26+O26</f>
+        <v>252</v>
+      </c>
+      <c r="X26">
+        <f t="shared" ref="X26:X27" si="19">W26/$W$27*100</f>
+        <v>53.05263157894737</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="G27" s="1">
+        <f>SUM(G25:G26)</f>
+        <v>456</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="16"/>
+        <v>100</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>100</v>
+      </c>
+      <c r="O27" s="1">
+        <f>SUM(O25:O26)</f>
+        <v>15</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="17"/>
+        <v>100</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="18"/>
+        <v>475</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="19"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="W32" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="X32" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>97</v>
+      </c>
+      <c r="D33">
+        <f>C33/$C$35*100</f>
+        <v>59.146341463414629</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>11</v>
+      </c>
+      <c r="H33">
+        <f>G33/$G$35*100</f>
+        <v>84.615384615384613</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>50</v>
+      </c>
+      <c r="V33" s="7">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <f>C33+G33+K33</f>
+        <v>109</v>
+      </c>
+      <c r="X33">
+        <f>W33/$W$35*100</f>
+        <v>60.893854748603346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B34" s="4">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>67</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:D35" si="20">C34/$C$35*100</f>
+        <v>40.853658536585364</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:H35" si="21">G34/$G$35*100</f>
+        <v>15.384615384615385</v>
+      </c>
+      <c r="J34" s="4">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>50</v>
+      </c>
+      <c r="V34" s="7">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <f t="shared" ref="W34:W35" si="22">C34+G34+K34</f>
+        <v>70</v>
+      </c>
+      <c r="X34">
+        <f t="shared" ref="X34:X35" si="23">W34/$W$35*100</f>
+        <v>39.106145251396647</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="C35" s="1">
+        <f>SUM(C33:C34)</f>
+        <v>164</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="20"/>
+        <v>100</v>
+      </c>
+      <c r="G35" s="1">
+        <f>SUM(G33:G34)</f>
+        <v>13</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="21"/>
+        <v>100</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>100</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="22"/>
+        <v>179</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="23"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X40" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B41" s="7">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f>C3+C10+C17</f>
+        <v>255</v>
+      </c>
+      <c r="D41">
+        <f>C41/$C$43*100</f>
+        <v>54.140127388535028</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>234</v>
+      </c>
+      <c r="H41">
+        <f>G41/$G$5*100</f>
+        <v>78.523489932885909</v>
+      </c>
+      <c r="J41" s="7">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f>K3+G10+G17+C25</f>
+        <v>492</v>
+      </c>
+      <c r="L41">
+        <f>K41/$K$43*100</f>
+        <v>66.757123473541384</v>
+      </c>
+      <c r="N41" s="7">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f>O3+K10+K17+G25+C33</f>
+        <v>1233</v>
+      </c>
+      <c r="P41">
+        <f>O41/$O$43*100</f>
+        <v>52.692307692307693</v>
+      </c>
+      <c r="R41" s="7">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <f>O10+O17+K25+G33</f>
+        <v>196</v>
+      </c>
+      <c r="T41">
+        <f>S41/$S$43*100</f>
+        <v>57.988165680473372</v>
+      </c>
+      <c r="V41" s="7">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <f>S3+O25+K33</f>
+        <v>46</v>
+      </c>
+      <c r="X41">
+        <f>W41/$W$43*100</f>
+        <v>62.162162162162161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:C43" si="24">C4+C11+C18</f>
+        <v>216</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:D43" si="25">C42/$C$43*100</f>
+        <v>45.859872611464972</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>64</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42:H43" si="26">G42/$G$5*100</f>
+        <v>21.476510067114095</v>
+      </c>
+      <c r="J42" s="7">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ref="K42:K43" si="27">K4+G11+G18+C26</f>
+        <v>245</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ref="L42:L43" si="28">K42/$K$43*100</f>
+        <v>33.242876526458616</v>
+      </c>
+      <c r="N42" s="7">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ref="O42:O43" si="29">O4+K11+K18+G26+C34</f>
+        <v>1107</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ref="P42:P43" si="30">O42/$O$43*100</f>
+        <v>47.307692307692307</v>
+      </c>
+      <c r="R42" s="7">
+        <v>1</v>
+      </c>
+      <c r="S42">
+        <f t="shared" ref="S42:S43" si="31">O11+O18+K26+G34</f>
+        <v>142</v>
+      </c>
+      <c r="T42">
+        <f t="shared" ref="T42:T43" si="32">S42/$S$43*100</f>
+        <v>42.011834319526628</v>
+      </c>
+      <c r="V42" s="7">
+        <v>1</v>
+      </c>
+      <c r="W42">
+        <f>S4+O26+K34</f>
+        <v>28</v>
+      </c>
+      <c r="X42">
+        <f t="shared" ref="X42:X43" si="33">W42/$W$43*100</f>
+        <v>37.837837837837839</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <f t="shared" si="24"/>
+        <v>471</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="25"/>
+        <v>100</v>
+      </c>
+      <c r="G43" s="1">
+        <f>SUM(G41:G42)</f>
+        <v>298</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="26"/>
+        <v>100</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="27"/>
+        <v>737</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="28"/>
+        <v>100</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="29"/>
+        <v>2340</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="30"/>
+        <v>100</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="31"/>
+        <v>338</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="32"/>
+        <v>100</v>
+      </c>
+      <c r="W43">
+        <f>S5+O27+K35</f>
+        <v>74</v>
+      </c>
+      <c r="X43">
+        <f t="shared" si="33"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="S47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="V47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="W47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z47" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="B48" s="7">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <f>G48+K48+O48+S48+W48</f>
+        <v>2456</v>
+      </c>
+      <c r="D48">
+        <f>C48/$C$50*100</f>
+        <v>57.67966181305777</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>957</v>
+      </c>
+      <c r="H48">
+        <v>65.682910089224436</v>
+      </c>
+      <c r="J48" s="7">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>590</v>
+      </c>
+      <c r="L48">
+        <v>56.840077071290942</v>
+      </c>
+      <c r="N48" s="7">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>577</v>
+      </c>
+      <c r="P48">
+        <v>52.028854824165919</v>
+      </c>
+      <c r="R48" s="7">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>223</v>
+      </c>
+      <c r="T48">
+        <v>46.94736842105263</v>
+      </c>
+      <c r="V48" s="7">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>109</v>
+      </c>
+      <c r="X48">
+        <v>60.893854748603346</v>
+      </c>
+      <c r="Z48" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <f>S48+W48</f>
+        <v>332</v>
+      </c>
+      <c r="AB48">
+        <f>AA48/$AA$50*100</f>
+        <v>50.764525993883794</v>
+      </c>
+    </row>
+    <row r="49" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B49" s="7">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:C50" si="34">G49+K49+O49+S49+W49</f>
+        <v>1802</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49:D50" si="35">C49/$C$50*100</f>
+        <v>42.320338186942223</v>
+      </c>
+      <c r="F49" s="7">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>500</v>
+      </c>
+      <c r="H49">
+        <v>34.317089910775564</v>
+      </c>
+      <c r="J49" s="7">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>448</v>
+      </c>
+      <c r="L49">
+        <v>43.159922928709058</v>
+      </c>
+      <c r="N49" s="7">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>532</v>
+      </c>
+      <c r="P49">
+        <v>47.971145175834081</v>
+      </c>
+      <c r="R49" s="7">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <v>252</v>
+      </c>
+      <c r="T49">
+        <v>53.05263157894737</v>
+      </c>
+      <c r="V49" s="7">
+        <v>1</v>
+      </c>
+      <c r="W49">
+        <v>70</v>
+      </c>
+      <c r="X49">
+        <v>39.106145251396647</v>
+      </c>
+      <c r="Z49" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" ref="AA49:AA50" si="36">S49+W49</f>
+        <v>322</v>
+      </c>
+      <c r="AB49">
+        <f t="shared" ref="AB49:AB50" si="37">AA49/$AA$50*100</f>
+        <v>49.235474006116206</v>
+      </c>
+    </row>
+    <row r="50" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="34"/>
+        <v>4258</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="35"/>
+        <v>100</v>
+      </c>
+      <c r="G50">
+        <v>1457</v>
+      </c>
+      <c r="H50">
+        <v>100</v>
+      </c>
+      <c r="K50">
+        <v>1038</v>
+      </c>
+      <c r="L50">
+        <v>100</v>
+      </c>
+      <c r="O50">
+        <v>1109</v>
+      </c>
+      <c r="P50">
+        <v>100</v>
+      </c>
+      <c r="S50">
+        <v>475</v>
+      </c>
+      <c r="T50">
+        <v>100</v>
+      </c>
+      <c r="W50">
+        <v>179</v>
+      </c>
+      <c r="X50">
+        <v>100</v>
+      </c>
+      <c r="AA50">
+        <f t="shared" si="36"/>
+        <v>654</v>
+      </c>
+      <c r="AB50">
+        <f t="shared" si="37"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5AACF4-39EA-4D0A-ACCC-8AAAEB1F46DD}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C56" activeCellId="36" sqref="C2 G2 K2 O2 S2 W2 S12 O12 K12 G12 C12 C21 G21 K21 O21 S21 S30 O30 K30 G30 C30 C39 G39 K39 O39 C48 G48 K48 O48 S48 W48 W56 S56 O56 K56 G56 C56"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2453,7 +3974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFBD1BB-8849-4487-8552-39BD208832CB}">
   <dimension ref="A1:X65"/>
   <sheetViews>
@@ -4692,11 +6213,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5BD43A-606A-44D1-B8DE-8471DD4CA647}">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V2" activeCellId="5" sqref="B2 F2 J2 N2 R2 V2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
comparison between cluster analysis clr-PCA
-exactly the same clusters are formed
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/1_groups_area_time.xlsx
+++ b/_CLUSTER/groups_time_area/1_groups_area_time.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_CLUSTER\groups_time_area\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6EE89F-6F2D-4087-AAC3-7C7AEC0B9FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4715B80-E79A-41DF-A4D8-6E091B22CCDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCF02780-D300-43E8-921C-29E8CAC5991E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BCF02780-D300-43E8-921C-29E8CAC5991E}"/>
   </bookViews>
   <sheets>
-    <sheet name="2_groups" sheetId="5" r:id="rId1"/>
-    <sheet name="3_groups" sheetId="1" r:id="rId2"/>
-    <sheet name="4_groups" sheetId="3" r:id="rId3"/>
-    <sheet name="6_groups" sheetId="4" r:id="rId4"/>
+    <sheet name="3_groups" sheetId="1" r:id="rId1"/>
+    <sheet name="4_groups" sheetId="3" r:id="rId2"/>
+    <sheet name="6_groups" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="50">
   <si>
     <t>Area1</t>
   </si>
@@ -187,21 +186,6 @@
   <si>
     <t>Area5_tot</t>
   </si>
-  <si>
-    <t>area1</t>
-  </si>
-  <si>
-    <t>area2</t>
-  </si>
-  <si>
-    <t>area3</t>
-  </si>
-  <si>
-    <t>Area_J</t>
-  </si>
-  <si>
-    <t>Area4+5</t>
-  </si>
 </sst>
 </file>
 
@@ -321,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -364,9 +348,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -680,1513 +661,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E362FAB3-749B-42AE-A5DF-A65E9F55F37B}">
-  <dimension ref="A1:AB50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA52" sqref="AA52"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="6.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" customWidth="1"/>
-    <col min="16" max="16" width="5.77734375" customWidth="1"/>
-    <col min="18" max="18" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" customWidth="1"/>
-    <col min="20" max="20" width="6.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>253</v>
-      </c>
-      <c r="D3">
-        <f>C3/$C$5*100</f>
-        <v>53.944562899786789</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>234</v>
-      </c>
-      <c r="H3">
-        <f>G3/$G$5*100</f>
-        <v>78.523489932885909</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>430</v>
-      </c>
-      <c r="L3">
-        <f>K3/$K$5*100</f>
-        <v>68.253968253968253</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
-      </c>
-      <c r="P3">
-        <v>100</v>
-      </c>
-      <c r="R3" s="4">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>37</v>
-      </c>
-      <c r="T3">
-        <f>S3/$S$5*100</f>
-        <v>64.912280701754383</v>
-      </c>
-      <c r="V3" s="7">
-        <v>0</v>
-      </c>
-      <c r="W3">
-        <f>C3+G3+K3+O3+S3</f>
-        <v>957</v>
-      </c>
-      <c r="X3">
-        <f>W3/$W$5*100</f>
-        <v>65.682910089224436</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>216</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D5" si="0">C4/$C$5*100</f>
-        <v>46.055437100213219</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>64</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H5" si="1">G4/$G$5*100</f>
-        <v>21.476510067114095</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>200</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L5" si="2">K4/$K$5*100</f>
-        <v>31.746031746031743</v>
-      </c>
-      <c r="N4" s="7">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>20</v>
-      </c>
-      <c r="T4">
-        <f t="shared" ref="T4:T5" si="3">S4/$S$5*100</f>
-        <v>35.087719298245609</v>
-      </c>
-      <c r="V4" s="7">
-        <v>1</v>
-      </c>
-      <c r="W4">
-        <f t="shared" ref="W4:W5" si="4">C4+G4+K4+O4+S4</f>
-        <v>500</v>
-      </c>
-      <c r="X4">
-        <f t="shared" ref="X4:X5" si="5">W4/$W$5*100</f>
-        <v>34.317089910775564</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C5" s="1">
-        <f>SUM(C3:C4)</f>
-        <v>469</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G5" s="1">
-        <f>SUM(G3:G4)</f>
-        <v>298</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="K5" s="1">
-        <f>SUM(K3:K4)</f>
-        <v>630</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5">
-        <v>100</v>
-      </c>
-      <c r="S5" s="1">
-        <f>SUM(S3:S4)</f>
-        <v>57</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="4"/>
-        <v>1457</v>
-      </c>
-      <c r="X5">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="W9" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="X9" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>100</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <f>G10/$G$12*100</f>
-        <v>71.428571428571431</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>406</v>
-      </c>
-      <c r="L10">
-        <f>K10/$K$12*100</f>
-        <v>56.783216783216787</v>
-      </c>
-      <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>178</v>
-      </c>
-      <c r="P10">
-        <f>O10/$O$12*100</f>
-        <v>56.507936507936506</v>
-      </c>
-      <c r="V10" s="7">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <f>C10+G10+K10+O10</f>
-        <v>590</v>
-      </c>
-      <c r="X10">
-        <f>W10/$W$12*100</f>
-        <v>56.840077071290942</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B11" s="7">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ref="H11:H12" si="6">G11/$G$12*100</f>
-        <v>28.571428571428569</v>
-      </c>
-      <c r="J11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>309</v>
-      </c>
-      <c r="L11">
-        <f t="shared" ref="L11:L12" si="7">K11/$K$12*100</f>
-        <v>43.216783216783213</v>
-      </c>
-      <c r="N11" s="4">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>137</v>
-      </c>
-      <c r="P11">
-        <f t="shared" ref="P11:P12" si="8">O11/$O$12*100</f>
-        <v>43.492063492063494</v>
-      </c>
-      <c r="V11" s="7">
-        <v>1</v>
-      </c>
-      <c r="W11">
-        <f t="shared" ref="W11:W12" si="9">C11+G11+K11+O11</f>
-        <v>448</v>
-      </c>
-      <c r="X11">
-        <f t="shared" ref="X11:X12" si="10">W11/$W$12*100</f>
-        <v>43.159922928709058</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="G12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="K12" s="1">
-        <f>SUM(K10:K11)</f>
-        <v>715</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="O12" s="1">
-        <f>SUM(O10:O11)</f>
-        <v>315</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="9"/>
-        <v>1038</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="W16" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="X16" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>100</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>57</v>
-      </c>
-      <c r="H17">
-        <f>G17/$G$19*100</f>
-        <v>57.575757575757578</v>
-      </c>
-      <c r="J17" s="4">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>513</v>
-      </c>
-      <c r="L17">
-        <f>K17/$K$19*100</f>
-        <v>51.197604790419163</v>
-      </c>
-      <c r="N17" s="4">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>6</v>
-      </c>
-      <c r="P17">
-        <f>O17/$O$19*100</f>
-        <v>85.714285714285708</v>
-      </c>
-      <c r="V17" s="7">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <f>C17+G17+K17+O17</f>
-        <v>577</v>
-      </c>
-      <c r="X17">
-        <f>W17/$W$19*100</f>
-        <v>52.028854824165919</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>42</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ref="H18:H19" si="11">G18/$G$19*100</f>
-        <v>42.424242424242422</v>
-      </c>
-      <c r="J18" s="4">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <v>489</v>
-      </c>
-      <c r="L18">
-        <f t="shared" ref="L18:L19" si="12">K18/$K$19*100</f>
-        <v>48.802395209580837</v>
-      </c>
-      <c r="N18" s="4">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <f t="shared" ref="P18:P19" si="13">O18/$O$19*100</f>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="V18" s="7">
-        <v>1</v>
-      </c>
-      <c r="W18">
-        <f t="shared" ref="W18:W19" si="14">C18+G18+K18+O18</f>
-        <v>532</v>
-      </c>
-      <c r="X18">
-        <f t="shared" ref="X18:X19" si="15">W18/$W$19*100</f>
-        <v>47.971145175834081</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>100</v>
-      </c>
-      <c r="G19" s="1">
-        <f>SUM(G17:G18)</f>
-        <v>99</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="11"/>
-        <v>100</v>
-      </c>
-      <c r="K19" s="1">
-        <f>SUM(K17:K18)</f>
-        <v>1002</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="12"/>
-        <v>100</v>
-      </c>
-      <c r="O19" s="1">
-        <f>SUM(O17:O18)</f>
-        <v>7</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="13"/>
-        <v>100</v>
-      </c>
-      <c r="W19">
-        <f t="shared" si="14"/>
-        <v>1109</v>
-      </c>
-      <c r="X19">
-        <f t="shared" si="15"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O24" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="P24" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="W24" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="X24" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B25" s="7">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>214</v>
-      </c>
-      <c r="H25">
-        <f>G25/$G$27*100</f>
-        <v>46.929824561403507</v>
-      </c>
-      <c r="J25" s="4">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>33.33</v>
-      </c>
-      <c r="N25" s="4">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>8</v>
-      </c>
-      <c r="P25">
-        <f>O25/$O$27*100</f>
-        <v>53.333333333333336</v>
-      </c>
-      <c r="V25" s="7">
-        <v>0</v>
-      </c>
-      <c r="W25">
-        <f>C25+G25+K25+O25</f>
-        <v>223</v>
-      </c>
-      <c r="X25">
-        <f>W25/$W$27*100</f>
-        <v>46.94736842105263</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>100</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>242</v>
-      </c>
-      <c r="H26">
-        <f t="shared" ref="H26:H27" si="16">G26/$G$27*100</f>
-        <v>53.070175438596493</v>
-      </c>
-      <c r="J26" s="4">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
-      <c r="L26">
-        <v>66.67</v>
-      </c>
-      <c r="N26" s="4">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <v>7</v>
-      </c>
-      <c r="P26">
-        <f t="shared" ref="P26:P27" si="17">O26/$O$27*100</f>
-        <v>46.666666666666664</v>
-      </c>
-      <c r="V26" s="7">
-        <v>1</v>
-      </c>
-      <c r="W26">
-        <f t="shared" ref="W26:W27" si="18">C26+G26+K26+O26</f>
-        <v>252</v>
-      </c>
-      <c r="X26">
-        <f t="shared" ref="X26:X27" si="19">W26/$W$27*100</f>
-        <v>53.05263157894737</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>100</v>
-      </c>
-      <c r="G27" s="1">
-        <f>SUM(G25:G26)</f>
-        <v>456</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="16"/>
-        <v>100</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-      <c r="L27">
-        <v>100</v>
-      </c>
-      <c r="O27" s="1">
-        <f>SUM(O25:O26)</f>
-        <v>15</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="17"/>
-        <v>100</v>
-      </c>
-      <c r="W27">
-        <f t="shared" si="18"/>
-        <v>475</v>
-      </c>
-      <c r="X27">
-        <f t="shared" si="19"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K32" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="W32" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="X32" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B33" s="4">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>97</v>
-      </c>
-      <c r="D33">
-        <f>C33/$C$35*100</f>
-        <v>59.146341463414629</v>
-      </c>
-      <c r="F33" s="4">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>11</v>
-      </c>
-      <c r="H33">
-        <f>G33/$G$35*100</f>
-        <v>84.615384615384613</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
-        <v>50</v>
-      </c>
-      <c r="V33" s="7">
-        <v>0</v>
-      </c>
-      <c r="W33">
-        <f>C33+G33+K33</f>
-        <v>109</v>
-      </c>
-      <c r="X33">
-        <f>W33/$W$35*100</f>
-        <v>60.893854748603346</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>67</v>
-      </c>
-      <c r="D34">
-        <f t="shared" ref="D34:D35" si="20">C34/$C$35*100</f>
-        <v>40.853658536585364</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
-      <c r="H34">
-        <f t="shared" ref="H34:H35" si="21">G34/$G$35*100</f>
-        <v>15.384615384615385</v>
-      </c>
-      <c r="J34" s="4">
-        <v>1</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34">
-        <v>50</v>
-      </c>
-      <c r="V34" s="7">
-        <v>1</v>
-      </c>
-      <c r="W34">
-        <f t="shared" ref="W34:W35" si="22">C34+G34+K34</f>
-        <v>70</v>
-      </c>
-      <c r="X34">
-        <f t="shared" ref="X34:X35" si="23">W34/$W$35*100</f>
-        <v>39.106145251396647</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="C35" s="1">
-        <f>SUM(C33:C34)</f>
-        <v>164</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="20"/>
-        <v>100</v>
-      </c>
-      <c r="G35" s="1">
-        <f>SUM(G33:G34)</f>
-        <v>13</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="21"/>
-        <v>100</v>
-      </c>
-      <c r="K35">
-        <v>2</v>
-      </c>
-      <c r="L35">
-        <v>100</v>
-      </c>
-      <c r="W35">
-        <f t="shared" si="22"/>
-        <v>179</v>
-      </c>
-      <c r="X35">
-        <f t="shared" si="23"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B40" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="N40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O40" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="P40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="R40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="S40" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="V40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="W40" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X40" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B41" s="7">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <f>C3+C10+C17</f>
-        <v>255</v>
-      </c>
-      <c r="D41">
-        <f>C41/$C$43*100</f>
-        <v>54.140127388535028</v>
-      </c>
-      <c r="F41" s="4">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>234</v>
-      </c>
-      <c r="H41">
-        <f>G41/$G$5*100</f>
-        <v>78.523489932885909</v>
-      </c>
-      <c r="J41" s="7">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <f>K3+G10+G17+C25</f>
-        <v>492</v>
-      </c>
-      <c r="L41">
-        <f>K41/$K$43*100</f>
-        <v>66.757123473541384</v>
-      </c>
-      <c r="N41" s="7">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <f>O3+K10+K17+G25+C33</f>
-        <v>1233</v>
-      </c>
-      <c r="P41">
-        <f>O41/$O$43*100</f>
-        <v>52.692307692307693</v>
-      </c>
-      <c r="R41" s="7">
-        <v>0</v>
-      </c>
-      <c r="S41">
-        <f>O10+O17+K25+G33</f>
-        <v>196</v>
-      </c>
-      <c r="T41">
-        <f>S41/$S$43*100</f>
-        <v>57.988165680473372</v>
-      </c>
-      <c r="V41" s="7">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <f>S3+O25+K33</f>
-        <v>46</v>
-      </c>
-      <c r="X41">
-        <f>W41/$W$43*100</f>
-        <v>62.162162162162161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B42" s="7">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <f t="shared" ref="C42:C43" si="24">C4+C11+C18</f>
-        <v>216</v>
-      </c>
-      <c r="D42">
-        <f t="shared" ref="D42:D43" si="25">C42/$C$43*100</f>
-        <v>45.859872611464972</v>
-      </c>
-      <c r="F42" s="4">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>64</v>
-      </c>
-      <c r="H42">
-        <f t="shared" ref="H42:H43" si="26">G42/$G$5*100</f>
-        <v>21.476510067114095</v>
-      </c>
-      <c r="J42" s="7">
-        <v>1</v>
-      </c>
-      <c r="K42">
-        <f t="shared" ref="K42:K43" si="27">K4+G11+G18+C26</f>
-        <v>245</v>
-      </c>
-      <c r="L42">
-        <f t="shared" ref="L42:L43" si="28">K42/$K$43*100</f>
-        <v>33.242876526458616</v>
-      </c>
-      <c r="N42" s="7">
-        <v>1</v>
-      </c>
-      <c r="O42">
-        <f t="shared" ref="O42:O43" si="29">O4+K11+K18+G26+C34</f>
-        <v>1107</v>
-      </c>
-      <c r="P42">
-        <f t="shared" ref="P42:P43" si="30">O42/$O$43*100</f>
-        <v>47.307692307692307</v>
-      </c>
-      <c r="R42" s="7">
-        <v>1</v>
-      </c>
-      <c r="S42">
-        <f t="shared" ref="S42:S43" si="31">O11+O18+K26+G34</f>
-        <v>142</v>
-      </c>
-      <c r="T42">
-        <f t="shared" ref="T42:T43" si="32">S42/$S$43*100</f>
-        <v>42.011834319526628</v>
-      </c>
-      <c r="V42" s="7">
-        <v>1</v>
-      </c>
-      <c r="W42">
-        <f>S4+O26+K34</f>
-        <v>28</v>
-      </c>
-      <c r="X42">
-        <f t="shared" ref="X42:X43" si="33">W42/$W$43*100</f>
-        <v>37.837837837837839</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="C43">
-        <f t="shared" si="24"/>
-        <v>471</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="25"/>
-        <v>100</v>
-      </c>
-      <c r="G43" s="1">
-        <f>SUM(G41:G42)</f>
-        <v>298</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="26"/>
-        <v>100</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="27"/>
-        <v>737</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="28"/>
-        <v>100</v>
-      </c>
-      <c r="O43">
-        <f t="shared" si="29"/>
-        <v>2340</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="30"/>
-        <v>100</v>
-      </c>
-      <c r="S43">
-        <f t="shared" si="31"/>
-        <v>338</v>
-      </c>
-      <c r="T43">
-        <f t="shared" si="32"/>
-        <v>100</v>
-      </c>
-      <c r="W43">
-        <f>S5+O27+K35</f>
-        <v>74</v>
-      </c>
-      <c r="X43">
-        <f t="shared" si="33"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B47" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="N47" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="P47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="R47" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="V47" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="W47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X47" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z47" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA47" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB47" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B48" s="7">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <f>G48+K48+O48+S48+W48</f>
-        <v>2456</v>
-      </c>
-      <c r="D48">
-        <f>C48/$C$50*100</f>
-        <v>57.67966181305777</v>
-      </c>
-      <c r="F48" s="7">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>957</v>
-      </c>
-      <c r="H48">
-        <v>65.682910089224436</v>
-      </c>
-      <c r="J48" s="7">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>590</v>
-      </c>
-      <c r="L48">
-        <v>56.840077071290942</v>
-      </c>
-      <c r="N48" s="7">
-        <v>0</v>
-      </c>
-      <c r="O48">
-        <v>577</v>
-      </c>
-      <c r="P48">
-        <v>52.028854824165919</v>
-      </c>
-      <c r="R48" s="7">
-        <v>0</v>
-      </c>
-      <c r="S48">
-        <v>223</v>
-      </c>
-      <c r="T48">
-        <v>46.94736842105263</v>
-      </c>
-      <c r="V48" s="7">
-        <v>0</v>
-      </c>
-      <c r="W48">
-        <v>109</v>
-      </c>
-      <c r="X48">
-        <v>60.893854748603346</v>
-      </c>
-      <c r="Z48" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA48">
-        <f>S48+W48</f>
-        <v>332</v>
-      </c>
-      <c r="AB48">
-        <f>AA48/$AA$50*100</f>
-        <v>50.764525993883794</v>
-      </c>
-    </row>
-    <row r="49" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B49" s="7">
-        <v>1</v>
-      </c>
-      <c r="C49">
-        <f t="shared" ref="C49:C50" si="34">G49+K49+O49+S49+W49</f>
-        <v>1802</v>
-      </c>
-      <c r="D49">
-        <f t="shared" ref="D49:D50" si="35">C49/$C$50*100</f>
-        <v>42.320338186942223</v>
-      </c>
-      <c r="F49" s="7">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>500</v>
-      </c>
-      <c r="H49">
-        <v>34.317089910775564</v>
-      </c>
-      <c r="J49" s="7">
-        <v>1</v>
-      </c>
-      <c r="K49">
-        <v>448</v>
-      </c>
-      <c r="L49">
-        <v>43.159922928709058</v>
-      </c>
-      <c r="N49" s="7">
-        <v>1</v>
-      </c>
-      <c r="O49">
-        <v>532</v>
-      </c>
-      <c r="P49">
-        <v>47.971145175834081</v>
-      </c>
-      <c r="R49" s="7">
-        <v>1</v>
-      </c>
-      <c r="S49">
-        <v>252</v>
-      </c>
-      <c r="T49">
-        <v>53.05263157894737</v>
-      </c>
-      <c r="V49" s="7">
-        <v>1</v>
-      </c>
-      <c r="W49">
-        <v>70</v>
-      </c>
-      <c r="X49">
-        <v>39.106145251396647</v>
-      </c>
-      <c r="Z49" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA49">
-        <f t="shared" ref="AA49:AA50" si="36">S49+W49</f>
-        <v>322</v>
-      </c>
-      <c r="AB49">
-        <f t="shared" ref="AB49:AB50" si="37">AA49/$AA$50*100</f>
-        <v>49.235474006116206</v>
-      </c>
-    </row>
-    <row r="50" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C50">
-        <f t="shared" si="34"/>
-        <v>4258</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="35"/>
-        <v>100</v>
-      </c>
-      <c r="G50">
-        <v>1457</v>
-      </c>
-      <c r="H50">
-        <v>100</v>
-      </c>
-      <c r="K50">
-        <v>1038</v>
-      </c>
-      <c r="L50">
-        <v>100</v>
-      </c>
-      <c r="O50">
-        <v>1109</v>
-      </c>
-      <c r="P50">
-        <v>100</v>
-      </c>
-      <c r="S50">
-        <v>475</v>
-      </c>
-      <c r="T50">
-        <v>100</v>
-      </c>
-      <c r="W50">
-        <v>179</v>
-      </c>
-      <c r="X50">
-        <v>100</v>
-      </c>
-      <c r="AA50">
-        <f t="shared" si="36"/>
-        <v>654</v>
-      </c>
-      <c r="AB50">
-        <f t="shared" si="37"/>
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5AACF4-39EA-4D0A-ACCC-8AAAEB1F46DD}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" activeCellId="36" sqref="C2 G2 K2 O2 S2 W2 S12 O12 K12 G12 C12 C21 G21 K21 O21 S21 S30 O30 K30 G30 C30 C39 G39 K39 O39 C48 G48 K48 O48 S48 W48 W56 S56 O56 K56 G56 C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3974,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFBD1BB-8849-4487-8552-39BD208832CB}">
   <dimension ref="A1:X65"/>
   <sheetViews>
@@ -6213,11 +4692,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5BD43A-606A-44D1-B8DE-8471DD4CA647}">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V2" activeCellId="5" sqref="B2 F2 J2 N2 R2 V2"/>
     </sheetView>
   </sheetViews>

</xml_diff>